<commit_message>
v9.10.0: STEAM_LOCOMOTIVE_MODE see change log
</commit_message>
<xml_diff>
--- a/documentation/ESCLinearity.xlsx
+++ b/documentation/ESCLinearity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinsommer/Documents/Programmieren/GitHub/RC/Rc_Engine_Sound_ESP32/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinsommer/Documents/Programmieren/GitHub/RC/Rc_Engine_Sound_ESP32/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C1A545-E174-B74A-9BD7-E915430BD85D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E6BF54-8763-0042-A0DA-675094BC9D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="3720" windowWidth="35760" windowHeight="22060" xr2:uid="{4FBCA326-246A-4146-9C0B-D49D78FD6B33}"/>
+    <workbookView xWindow="22860" yWindow="3400" windowWidth="35760" windowHeight="22060" xr2:uid="{4FBCA326-246A-4146-9C0B-D49D78FD6B33}"/>
   </bookViews>
   <sheets>
     <sheet name="Quicrun Fusion" sheetId="1" r:id="rId1"/>
@@ -1764,7 +1764,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>